<commit_message>
Enhance declaration layout: Add flexbox styling for document content and quantities section, improve footer positioning, and update quantity display for better readability.
</commit_message>
<xml_diff>
--- a/data/clients.xlsx
+++ b/data/clients.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Clients" sheetId="1" r:id="rId1"/>
+    <sheet name="clients" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -432,9 +432,6 @@
       <c r="D2" t="str">
         <v>Antenne 1</v>
       </c>
-      <c r="E2" t="str">
-        <v>Point A, Point B, Point C</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -449,9 +446,6 @@
       <c r="D3" t="str">
         <v>Antenne 2</v>
       </c>
-      <c r="E3" t="str">
-        <v>Point D, Point E, Point F</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -466,9 +460,6 @@
       <c r="D4" t="str">
         <v>Test Antenne</v>
       </c>
-      <c r="E4" t="str">
-        <v>Start, Middle, End</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -483,9 +474,6 @@
       <c r="D5" t="str">
         <v>Antenne 3</v>
       </c>
-      <c r="E5" t="str">
-        <v>Route 1, Route 2</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -499,9 +487,6 @@
       </c>
       <c r="D6" t="str">
         <v>teat</v>
-      </c>
-      <c r="E6" t="str">
-        <v>w, e, r, ty</v>
       </c>
     </row>
   </sheetData>

</xml_diff>